<commit_message>
More IRR code changes
More IRR code changes
</commit_message>
<xml_diff>
--- a/inter_rater_reliability_results.xlsx
+++ b/inter_rater_reliability_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Projects/CoMSAfrica/Geneva/Data analysis/CoMSA_stats/comsafrica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4163D609-517C-F643-8466-769AEEA22780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E6F391-FC60-514D-8F87-887662FF40BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{FB42F035-823F-2442-986B-DBADFA145460}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{FB42F035-823F-2442-986B-DBADFA145460}"/>
   </bookViews>
   <sheets>
     <sheet name="Categorical variables" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
   <si>
     <t>Variable</t>
   </si>
@@ -176,12 +176,24 @@
   </si>
   <si>
     <t>Continuous</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>strange distribution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -234,28 +246,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,318 +591,317 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB72A55B-FC13-CA45-931E-F3F555C583F4}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="B1:G15"/>
   <sheetViews>
-    <sheetView zoomScale="252" zoomScaleNormal="252" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:7">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="2" spans="2:7">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="D2" s="8">
         <v>0.44590000000000002</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="8">
         <v>0.26329999999999998</v>
       </c>
-      <c r="E2">
+      <c r="F2" s="8">
         <v>0.63519999999999999</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+    <row r="3" spans="2:7">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="D3" s="8">
         <v>0.50939999999999996</v>
       </c>
-      <c r="D3">
+      <c r="E3" s="8">
         <v>0.33279999999999998</v>
       </c>
-      <c r="E3">
+      <c r="F3" s="8">
         <v>0.65269999999999995</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+    <row r="4" spans="2:7">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="D4" s="8">
         <v>0.17349999999999999</v>
       </c>
-      <c r="D4">
+      <c r="E4" s="8">
         <v>0.10979999999999999</v>
       </c>
-      <c r="E4">
+      <c r="F4" s="8">
         <v>0.25609999999999999</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+    <row r="5" spans="2:7">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="D5" s="8">
         <v>0.4551</v>
       </c>
-      <c r="D5">
+      <c r="E5" s="8">
         <v>0.34760000000000002</v>
       </c>
-      <c r="E5">
+      <c r="F5" s="8">
         <v>0.61380000000000001</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+    <row r="6" spans="2:7">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6">
+      <c r="D6" s="8">
         <v>0.1082</v>
       </c>
-      <c r="D6">
+      <c r="E6" s="8">
         <v>-9.1420000000000001E-2</v>
       </c>
-      <c r="E6">
+      <c r="F6" s="8">
         <v>0.28520000000000001</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
+    <row r="7" spans="2:7">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
+      <c r="D7" s="8">
         <v>0.56910000000000005</v>
       </c>
-      <c r="D7">
+      <c r="E7" s="8">
         <v>0.42170000000000002</v>
       </c>
-      <c r="E7">
+      <c r="F7" s="8">
         <v>0.73919999999999997</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+    <row r="8" spans="2:7">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="C8">
+      <c r="D8" s="8">
         <v>0.26919999999999999</v>
       </c>
-      <c r="D8">
+      <c r="E8" s="8">
         <v>0.15759999999999999</v>
       </c>
-      <c r="E8">
+      <c r="F8" s="8">
         <v>0.39329999999999998</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+    <row r="9" spans="2:7">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="C9">
+      <c r="D9" s="8">
         <v>0.10150000000000001</v>
       </c>
-      <c r="D9">
+      <c r="E9" s="8">
         <v>-0.56940000000000002</v>
       </c>
-      <c r="E9">
+      <c r="F9" s="8">
         <v>0.61699999999999999</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+    <row r="10" spans="2:7">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="C10">
+      <c r="D10" s="8">
         <v>0.18859999999999999</v>
       </c>
-      <c r="D10">
+      <c r="E10" s="8">
         <v>0.13589999999999999</v>
       </c>
-      <c r="E10">
+      <c r="F10" s="8">
         <v>0.25840000000000002</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
+    <row r="11" spans="2:7">
+      <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="C11">
+      <c r="D11" s="8">
         <v>0.3518</v>
       </c>
-      <c r="D11">
+      <c r="E11" s="8">
         <v>0.26790000000000003</v>
       </c>
-      <c r="E11">
+      <c r="F11" s="8">
         <v>0.4335</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
+    <row r="12" spans="2:7">
+      <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="C12">
+      <c r="D12" s="8">
         <v>0.3508</v>
       </c>
-      <c r="D12">
+      <c r="E12" s="8">
         <v>0.27710000000000001</v>
       </c>
-      <c r="E12">
+      <c r="F12" s="8">
         <v>0.43290000000000001</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
+    <row r="13" spans="2:7">
+      <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="C13">
+      <c r="D13" s="8">
         <v>0.30880000000000002</v>
       </c>
-      <c r="D13">
+      <c r="E13" s="8">
         <v>0.16969999999999999</v>
       </c>
-      <c r="E13">
+      <c r="F13" s="8">
         <v>0.45689999999999997</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
+    <row r="14" spans="2:7">
+      <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>18</v>
       </c>
-      <c r="C14">
+      <c r="D14" s="8">
         <v>0.14660000000000001</v>
       </c>
-      <c r="D14">
+      <c r="E14" s="8">
         <v>-0.29870000000000002</v>
       </c>
-      <c r="E14">
+      <c r="F14" s="8">
         <v>0.57540000000000002</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
+    <row r="15" spans="2:7">
+      <c r="B15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>20</v>
       </c>
-      <c r="C15">
+      <c r="D15" s="8">
         <v>0.33300000000000002</v>
       </c>
-      <c r="D15">
+      <c r="E15" s="8">
         <v>0.2535</v>
       </c>
-      <c r="E15">
+      <c r="F15" s="8">
         <v>0.41139999999999999</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>44</v>
       </c>
     </row>
@@ -892,514 +912,846 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFB3FF2-77B5-D244-AC2F-4BD444475F41}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="B2:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:9">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
+      <c r="I2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="9">
+      <c r="E3" s="6">
         <v>0.40200000000000002</v>
       </c>
-      <c r="E2" s="9">
+      <c r="F3" s="6">
         <v>0.19600000000000001</v>
       </c>
-      <c r="F2" s="9">
+      <c r="G3" s="6">
         <v>0.53300000000000003</v>
       </c>
-      <c r="G2" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4" t="s">
+      <c r="H3" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="13"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="9">
+      <c r="E4" s="6">
         <v>0.40200000000000002</v>
       </c>
-      <c r="E3" s="9">
+      <c r="F4" s="6">
         <v>0.15</v>
       </c>
-      <c r="F3" s="9">
+      <c r="G4" s="6">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G3" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4" t="s">
+      <c r="H4" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="13"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="9">
+      <c r="E5" s="6">
         <v>0.46400000000000002</v>
       </c>
-      <c r="E4" s="9">
+      <c r="F5" s="6">
         <v>0.161</v>
       </c>
-      <c r="F4" s="9">
+      <c r="G5" s="6">
         <v>0.69199999999999995</v>
       </c>
-      <c r="G4" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4" t="s">
+      <c r="H5" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="13"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="9">
+      <c r="E6" s="6">
         <v>0.54200000000000004</v>
       </c>
-      <c r="E5" s="9">
+      <c r="F6" s="6">
         <v>0.253</v>
       </c>
-      <c r="F5" s="9">
+      <c r="G6" s="6">
         <v>0.83799999999999997</v>
       </c>
-      <c r="G5" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="6" t="s">
+      <c r="H6" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="13"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="10">
+      <c r="E7" s="7">
         <v>0.73699999999999999</v>
       </c>
-      <c r="E6" s="10">
+      <c r="F7" s="7">
         <v>0.57299999999999995</v>
       </c>
-      <c r="F6" s="10">
+      <c r="G7" s="7">
         <v>0.83499999999999996</v>
       </c>
-      <c r="G6" s="6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="H7" s="4">
+        <v>50</v>
+      </c>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="13"/>
+      <c r="C8" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="11">
+      <c r="E8" s="6">
         <v>0.90900000000000003</v>
       </c>
-      <c r="E7" s="11">
+      <c r="F8" s="6">
         <v>0.86199999999999999</v>
       </c>
-      <c r="F7" s="11">
+      <c r="G8" s="6">
         <v>0.93600000000000005</v>
       </c>
-      <c r="G7" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="8" t="s">
+      <c r="H8" s="3">
+        <v>50</v>
+      </c>
+      <c r="I8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="13"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="11">
+      <c r="E9" s="6">
         <v>0.97899999999999998</v>
       </c>
-      <c r="E8" s="11">
+      <c r="F9" s="6">
         <v>0.96799999999999997</v>
       </c>
-      <c r="F8" s="11">
+      <c r="G9" s="6">
         <v>0.98599999999999999</v>
       </c>
-      <c r="G8" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="8" t="s">
+      <c r="H9" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="13"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="11">
+      <c r="E10" s="14">
         <v>0.999</v>
       </c>
-      <c r="E9" s="11">
+      <c r="F10" s="14">
         <v>0.999</v>
       </c>
-      <c r="F9" s="11">
+      <c r="G10" s="14">
         <v>1</v>
       </c>
-      <c r="G9" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="8" t="s">
+      <c r="H10" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="13"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="11">
+      <c r="E11" s="6">
         <v>0.96499999999999997</v>
       </c>
-      <c r="E10" s="11">
+      <c r="F11" s="6">
         <v>0.94399999999999995</v>
       </c>
-      <c r="F10" s="11">
+      <c r="G11" s="6">
         <v>0.97499999999999998</v>
       </c>
-      <c r="G10" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="8" t="s">
+      <c r="H11" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="13"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="11">
+      <c r="E12" s="6">
         <v>0.89500000000000002</v>
       </c>
-      <c r="E11" s="11">
+      <c r="F12" s="6">
         <v>0.84099999999999997</v>
       </c>
-      <c r="F11" s="11">
+      <c r="G12" s="6">
         <v>0.92500000000000004</v>
       </c>
-      <c r="G11" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="8" t="s">
+      <c r="H12" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="13"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="11">
+      <c r="E13" s="6">
         <v>0.84299999999999997</v>
       </c>
-      <c r="E12" s="11">
+      <c r="F13" s="6">
         <v>0.77100000000000002</v>
       </c>
-      <c r="F12" s="11">
+      <c r="G13" s="6">
         <v>0.88700000000000001</v>
       </c>
-      <c r="G12" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="8" t="s">
+      <c r="H13" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="13"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="11">
+      <c r="E14" s="6">
         <v>0.88900000000000001</v>
       </c>
-      <c r="E13" s="11">
+      <c r="F14" s="6">
         <v>0.83599999999999997</v>
       </c>
-      <c r="F13" s="11">
+      <c r="G14" s="6">
         <v>0.92100000000000004</v>
       </c>
-      <c r="G13" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="8" t="s">
+      <c r="H14" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="13"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="11">
+      <c r="E15" s="6">
         <v>0.84599999999999997</v>
       </c>
-      <c r="E14" s="11">
+      <c r="F15" s="6">
         <v>0.77200000000000002</v>
       </c>
-      <c r="F14" s="11">
+      <c r="G15" s="6">
         <v>0.88800000000000001</v>
       </c>
-      <c r="G14" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="8" t="s">
+      <c r="H15" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="13"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="11">
+      <c r="E16" s="6">
         <v>0.88200000000000001</v>
       </c>
-      <c r="E15" s="11">
+      <c r="F16" s="6">
         <v>0.82499999999999996</v>
       </c>
-      <c r="F15" s="11">
+      <c r="G16" s="6">
         <v>0.91600000000000004</v>
       </c>
-      <c r="G15" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="8" t="s">
+      <c r="H16" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="13"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="11">
+      <c r="E17" s="6">
         <v>0.89300000000000002</v>
       </c>
-      <c r="E16" s="11">
+      <c r="F17" s="6">
         <v>0.83699999999999997</v>
       </c>
-      <c r="F16" s="11">
+      <c r="G17" s="6">
         <v>0.92600000000000005</v>
       </c>
-      <c r="G16" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="8" t="s">
+      <c r="H17" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="13"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="11">
+      <c r="E18" s="6">
         <v>0.82899999999999996</v>
       </c>
-      <c r="E17" s="11">
+      <c r="F18" s="6">
         <v>0.752</v>
       </c>
-      <c r="F17" s="11">
+      <c r="G18" s="6">
         <v>0.877</v>
       </c>
-      <c r="G17" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="8" t="s">
+      <c r="H18" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="13"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="11">
+      <c r="E19" s="6">
         <v>0.86399999999999999</v>
       </c>
-      <c r="E18" s="11">
+      <c r="F19" s="6">
         <v>0.8</v>
       </c>
-      <c r="F18" s="11">
+      <c r="G19" s="6">
         <v>0.90400000000000003</v>
       </c>
-      <c r="G18" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="8" t="s">
+      <c r="H19" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="13"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="11">
+      <c r="E20" s="6">
         <v>0.88200000000000001</v>
       </c>
-      <c r="E19" s="11">
+      <c r="F20" s="6">
         <v>0.82499999999999996</v>
       </c>
-      <c r="F19" s="11">
+      <c r="G20" s="6">
         <v>0.91700000000000004</v>
       </c>
-      <c r="G19" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="8" t="s">
+      <c r="H20" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="13"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="11">
+      <c r="E21" s="6">
         <v>0.82199999999999995</v>
       </c>
-      <c r="E20" s="11">
+      <c r="F21" s="6">
         <v>0.73899999999999999</v>
       </c>
-      <c r="F20" s="11">
+      <c r="G21" s="6">
         <v>0.87</v>
       </c>
-      <c r="G20" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="8" t="s">
+      <c r="H21" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="13"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="11">
+      <c r="E22" s="6">
         <v>0.83199999999999996</v>
       </c>
-      <c r="E21" s="11">
+      <c r="F22" s="6">
         <v>0.754</v>
       </c>
-      <c r="F21" s="11">
+      <c r="G22" s="6">
         <v>0.878</v>
       </c>
-      <c r="G21" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="8" t="s">
+      <c r="H22" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="13"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="11">
+      <c r="E23" s="6">
         <v>0.80800000000000005</v>
       </c>
-      <c r="E22" s="11">
+      <c r="F23" s="6">
         <v>0.72599999999999998</v>
       </c>
-      <c r="F22" s="11">
+      <c r="G23" s="6">
         <v>0.86</v>
       </c>
-      <c r="G22" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="8" t="s">
+      <c r="H23" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="15"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="11">
+      <c r="E24" s="7">
         <v>1.6900000000000001E-3</v>
       </c>
-      <c r="E23" s="11">
+      <c r="F24" s="7">
         <v>0</v>
       </c>
-      <c r="F23" s="11">
+      <c r="G24" s="7">
         <v>5.0599999999999999E-2</v>
       </c>
-      <c r="G23" s="4">
-        <v>50</v>
+      <c r="H24" s="4">
+        <v>50</v>
+      </c>
+      <c r="I24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="6">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="H25" s="17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="13"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="H26" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="13"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="H27" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="13"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="6">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0.222</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="H28" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="13"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="H29" s="16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="G30" s="8">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="I30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="12"/>
+      <c r="D31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="G31" s="8">
+        <v>0.98699999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="12"/>
+      <c r="D32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="8">
+        <v>1</v>
+      </c>
+      <c r="F32" s="8">
+        <v>1</v>
+      </c>
+      <c r="G32" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="12"/>
+      <c r="D33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="8">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="F33" s="8">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="G33" s="8">
+        <v>0.96599999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="12"/>
+      <c r="D34" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="8">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="G34" s="8">
+        <v>0.93899999999999995</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="12"/>
+      <c r="D35" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="8">
+        <v>0.753</v>
+      </c>
+      <c r="F35" s="8">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="G35" s="8">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="12"/>
+      <c r="D36" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="8">
+        <v>0.755</v>
+      </c>
+      <c r="F36" s="8">
+        <v>0.66</v>
+      </c>
+      <c r="G36" s="8">
+        <v>0.82099999999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="12"/>
+      <c r="D37" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" s="8">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="F37" s="8">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="G37" s="8">
+        <v>0.88300000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="12"/>
+      <c r="D38" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="8">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="F38" s="8">
+        <v>0.66</v>
+      </c>
+      <c r="G38" s="8">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="12"/>
+      <c r="D39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="8">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="F39" s="8">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="G39" s="8">
+        <v>0.83299999999999996</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="12"/>
+      <c r="D40" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="8">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="F40" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="G40" s="8">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="12"/>
+      <c r="D41" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="8">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="F41" s="8">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="G41" s="8">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" s="12"/>
+      <c r="D42" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="F42" s="8">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="G42" s="8">
+        <v>0.91500000000000004</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="12"/>
+      <c r="D43" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" s="8">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="F43" s="8">
+        <v>0.745</v>
+      </c>
+      <c r="G43" s="8">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" s="12"/>
+      <c r="D44" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="8">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0.72</v>
+      </c>
+      <c r="G44" s="8">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="B45" s="12"/>
+      <c r="D45" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" s="8">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="F45" s="8">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="G45" s="8">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="B46" s="12"/>
+      <c r="D46" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" s="8">
+        <v>8.1199999999999994E-2</v>
+      </c>
+      <c r="F46" s="8">
+        <v>1.78E-2</v>
+      </c>
+      <c r="G46" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="I46" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="B7:B23"/>
+  <mergeCells count="4">
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="C8:C24"/>
+    <mergeCell ref="B30:B46"/>
+    <mergeCell ref="C25:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added summary code for FLK_FORM and RED_TYP
Added summary code for FLK_FORM and RED_TYP and updated excel spreadsheet results
</commit_message>
<xml_diff>
--- a/inter_rater_reliability_results.xlsx
+++ b/inter_rater_reliability_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Projects/CoMSAfrica/Geneva/Data analysis/CoMSA_stats/comsafrica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DB40D9-A0E0-0A4B-9C78-78B4BB4E6AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9484D4-A498-8745-850E-5C4DBF6887DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{FB42F035-823F-2442-986B-DBADFA145460}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{FB42F035-823F-2442-986B-DBADFA145460}"/>
   </bookViews>
   <sheets>
     <sheet name="Categorical variables" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="129">
   <si>
     <t>Variable</t>
   </si>
@@ -405,6 +405,24 @@
   </si>
   <si>
     <t>Fleiss' Kappa</t>
+  </si>
+  <si>
+    <t>Flake form</t>
+  </si>
+  <si>
+    <t>Blade</t>
+  </si>
+  <si>
+    <t>Convflake</t>
+  </si>
+  <si>
+    <t>Flake</t>
+  </si>
+  <si>
+    <t>Indet</t>
+  </si>
+  <si>
+    <t>Reduction system</t>
   </si>
 </sst>
 </file>
@@ -414,7 +432,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -432,6 +450,11 @@
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="TimesNewRomanPSMT"/>
     </font>
   </fonts>
   <fills count="2">
@@ -481,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -494,15 +517,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -513,6 +527,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,14 +568,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>482863</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>99219</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>162982</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>70308</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>70309</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -937,11 +969,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB72A55B-FC13-CA45-931E-F3F555C583F4}">
-  <dimension ref="B1:I29"/>
+  <dimension ref="B1:I33"/>
   <sheetViews>
-    <sheetView zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -952,67 +984,64 @@
     <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:9" ht="17" thickBot="1">
+      <c r="B1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="2:9">
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="8">
-        <v>0.44590000000000002</v>
-      </c>
-      <c r="E2" s="8">
-        <v>0.26329999999999998</v>
-      </c>
-      <c r="F2" s="8">
-        <v>0.63519999999999999</v>
-      </c>
-      <c r="G2">
-        <v>49</v>
-      </c>
-      <c r="I2" t="s">
-        <v>121</v>
+      <c r="B2" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="31">
+        <v>0.1116</v>
+      </c>
+      <c r="E2" s="31">
+        <v>-7.9399999999999998E-2</v>
+      </c>
+      <c r="F2" s="31">
+        <v>0.33019999999999999</v>
+      </c>
+      <c r="G2" s="33">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:9">
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0.50939999999999996</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0.33279999999999998</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.65269999999999995</v>
-      </c>
-      <c r="G3">
-        <v>48</v>
+      <c r="B3" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="25">
+        <v>0.4597</v>
+      </c>
+      <c r="E3" s="26">
+        <v>0.30630000000000002</v>
+      </c>
+      <c r="F3" s="26">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="G3" s="25">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="2:9">
@@ -1020,19 +1049,22 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="8">
-        <v>0.17349999999999999</v>
+        <v>0.44590000000000002</v>
       </c>
       <c r="E4" s="8">
-        <v>0.10979999999999999</v>
+        <v>0.26329999999999998</v>
       </c>
       <c r="F4" s="8">
-        <v>0.25609999999999999</v>
+        <v>0.63519999999999999</v>
       </c>
       <c r="G4">
-        <v>44</v>
+        <v>49</v>
+      </c>
+      <c r="I4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="2:9">
@@ -1040,19 +1072,19 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" s="8">
-        <v>0.4551</v>
+        <v>0.50939999999999996</v>
       </c>
       <c r="E5" s="8">
-        <v>0.34760000000000002</v>
+        <v>0.33279999999999998</v>
       </c>
       <c r="F5" s="8">
-        <v>0.61380000000000001</v>
+        <v>0.65269999999999995</v>
       </c>
       <c r="G5">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:9">
@@ -1060,19 +1092,19 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="8">
-        <v>0.1082</v>
+        <v>0.17349999999999999</v>
       </c>
       <c r="E6" s="8">
-        <v>-9.1420000000000001E-2</v>
+        <v>0.10979999999999999</v>
       </c>
       <c r="F6" s="8">
-        <v>0.28520000000000001</v>
+        <v>0.25609999999999999</v>
       </c>
       <c r="G6">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="2:9">
@@ -1080,19 +1112,19 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="8">
-        <v>0.56910000000000005</v>
+        <v>0.4551</v>
       </c>
       <c r="E7" s="8">
-        <v>0.42170000000000002</v>
+        <v>0.34760000000000002</v>
       </c>
       <c r="F7" s="8">
-        <v>0.73919999999999997</v>
+        <v>0.61380000000000001</v>
       </c>
       <c r="G7">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="2:9">
@@ -1100,19 +1132,19 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="8">
-        <v>0.26919999999999999</v>
+        <v>0.1082</v>
       </c>
       <c r="E8" s="8">
-        <v>0.15759999999999999</v>
+        <v>-9.1420000000000001E-2</v>
       </c>
       <c r="F8" s="8">
-        <v>0.39329999999999998</v>
+        <v>0.28520000000000001</v>
       </c>
       <c r="G8">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:9">
@@ -1120,16 +1152,16 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D9" s="8">
-        <v>0.10150000000000001</v>
+        <v>0.56910000000000005</v>
       </c>
       <c r="E9" s="8">
-        <v>-0.56940000000000002</v>
+        <v>0.42170000000000002</v>
       </c>
       <c r="F9" s="8">
-        <v>0.61699999999999999</v>
+        <v>0.73919999999999997</v>
       </c>
       <c r="G9">
         <v>47</v>
@@ -1140,19 +1172,19 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" s="8">
-        <v>0.18859999999999999</v>
+        <v>0.26919999999999999</v>
       </c>
       <c r="E10" s="8">
-        <v>0.13589999999999999</v>
+        <v>0.15759999999999999</v>
       </c>
       <c r="F10" s="8">
-        <v>0.25840000000000002</v>
+        <v>0.39329999999999998</v>
       </c>
       <c r="G10">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -1160,19 +1192,19 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" s="8">
-        <v>0.3518</v>
+        <v>0.10150000000000001</v>
       </c>
       <c r="E11" s="8">
-        <v>0.26790000000000003</v>
+        <v>-0.56940000000000002</v>
       </c>
       <c r="F11" s="8">
-        <v>0.4335</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="G11">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:9">
@@ -1180,19 +1212,19 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12" s="8">
-        <v>0.3508</v>
+        <v>0.18859999999999999</v>
       </c>
       <c r="E12" s="8">
-        <v>0.27710000000000001</v>
+        <v>0.13589999999999999</v>
       </c>
       <c r="F12" s="8">
-        <v>0.43290000000000001</v>
+        <v>0.25840000000000002</v>
       </c>
       <c r="G12">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:9">
@@ -1200,19 +1232,19 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13" s="8">
-        <v>0.30880000000000002</v>
+        <v>0.3518</v>
       </c>
       <c r="E13" s="8">
-        <v>0.16969999999999999</v>
+        <v>0.26790000000000003</v>
       </c>
       <c r="F13" s="8">
-        <v>0.45689999999999997</v>
+        <v>0.4335</v>
       </c>
       <c r="G13">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="2:9">
@@ -1220,119 +1252,119 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" s="8">
-        <v>0.14660000000000001</v>
+        <v>0.3508</v>
       </c>
       <c r="E14" s="8">
-        <v>-0.29870000000000002</v>
+        <v>0.27710000000000001</v>
       </c>
       <c r="F14" s="8">
-        <v>0.57540000000000002</v>
+        <v>0.43290000000000001</v>
       </c>
       <c r="G14">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:9">
-      <c r="B15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="7">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="E15" s="7">
-        <v>0.2535</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0.41139999999999999</v>
-      </c>
-      <c r="G15" s="4">
-        <v>44</v>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.30880000000000002</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.16969999999999999</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.45689999999999997</v>
+      </c>
+      <c r="G15">
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="2:9">
       <c r="B16" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D16" s="8">
-        <v>0.52749999999999997</v>
+        <v>0.14660000000000001</v>
       </c>
       <c r="E16" s="8">
-        <v>0.36890000000000001</v>
+        <v>-0.29870000000000002</v>
       </c>
       <c r="F16" s="8">
-        <v>0.69710000000000005</v>
+        <v>0.57540000000000002</v>
       </c>
       <c r="G16">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="8">
-        <v>0.64</v>
-      </c>
-      <c r="E17" s="8">
-        <v>0.4758</v>
-      </c>
-      <c r="F17" s="8">
-        <v>0.81159999999999999</v>
-      </c>
-      <c r="G17">
-        <v>50</v>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.2535</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.41139999999999999</v>
+      </c>
+      <c r="G17" s="4">
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0.1741</v>
-      </c>
-      <c r="E18" s="8">
-        <v>0.11650000000000001</v>
-      </c>
-      <c r="F18" s="8">
-        <v>0.23719999999999999</v>
-      </c>
-      <c r="G18">
-        <v>47</v>
+      <c r="B18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0.31929999999999997</v>
+      </c>
+      <c r="E18" s="6">
+        <v>0.19420000000000001</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0.46110000000000001</v>
+      </c>
+      <c r="G18" s="27">
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0.38769999999999999</v>
-      </c>
-      <c r="E19" s="8">
-        <v>0.29010000000000002</v>
-      </c>
-      <c r="F19" s="8">
-        <v>0.46610000000000001</v>
-      </c>
-      <c r="G19">
-        <v>47</v>
+      <c r="B19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.32729999999999998</v>
+      </c>
+      <c r="E19" s="6">
+        <v>0.1396</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0.54749999999999999</v>
+      </c>
+      <c r="G19" s="12">
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:7">
@@ -1340,19 +1372,19 @@
         <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D20" s="8">
-        <v>0.1109</v>
+        <v>0.52749999999999997</v>
       </c>
       <c r="E20" s="8">
-        <v>-0.158</v>
+        <v>0.36890000000000001</v>
       </c>
       <c r="F20" s="8">
-        <v>0.3609</v>
+        <v>0.69710000000000005</v>
       </c>
       <c r="G20">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="2:7">
@@ -1360,16 +1392,16 @@
         <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D21" s="8">
-        <v>0.38669999999999999</v>
+        <v>0.64</v>
       </c>
       <c r="E21" s="8">
-        <v>0.19239999999999999</v>
+        <v>0.4758</v>
       </c>
       <c r="F21" s="8">
-        <v>0.59140000000000004</v>
+        <v>0.81159999999999999</v>
       </c>
       <c r="G21">
         <v>50</v>
@@ -1380,19 +1412,19 @@
         <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D22" s="8">
-        <v>0.28949999999999998</v>
+        <v>0.1741</v>
       </c>
       <c r="E22" s="8">
-        <v>0.17119999999999999</v>
+        <v>0.11650000000000001</v>
       </c>
       <c r="F22" s="8">
-        <v>0.41670000000000001</v>
+        <v>0.23719999999999999</v>
       </c>
       <c r="G22">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="2:7">
@@ -1400,19 +1432,19 @@
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D23" s="8">
-        <v>8.4959999999999994E-2</v>
+        <v>0.38769999999999999</v>
       </c>
       <c r="E23" s="8">
-        <v>-0.439</v>
+        <v>0.29010000000000002</v>
       </c>
       <c r="F23" s="8">
-        <v>0.59489999999999998</v>
+        <v>0.46610000000000001</v>
       </c>
       <c r="G23">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="2:7">
@@ -1420,16 +1452,16 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D24" s="8">
-        <v>0.1037</v>
+        <v>0.1109</v>
       </c>
       <c r="E24" s="8">
-        <v>5.2440000000000001E-2</v>
+        <v>-0.158</v>
       </c>
       <c r="F24" s="8">
-        <v>0.1555</v>
+        <v>0.3609</v>
       </c>
       <c r="G24">
         <v>47</v>
@@ -1440,16 +1472,16 @@
         <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D25" s="8">
-        <v>0.28999999999999998</v>
+        <v>0.38669999999999999</v>
       </c>
       <c r="E25" s="8">
-        <v>0.1905</v>
+        <v>0.19239999999999999</v>
       </c>
       <c r="F25" s="8">
-        <v>0.38300000000000001</v>
+        <v>0.59140000000000004</v>
       </c>
       <c r="G25">
         <v>50</v>
@@ -1460,19 +1492,19 @@
         <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D26" s="8">
-        <v>0.34770000000000001</v>
+        <v>0.28949999999999998</v>
       </c>
       <c r="E26" s="8">
-        <v>0.29160000000000003</v>
+        <v>0.17119999999999999</v>
       </c>
       <c r="F26" s="8">
-        <v>0.42420000000000002</v>
+        <v>0.41670000000000001</v>
       </c>
       <c r="G26">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="2:7">
@@ -1480,19 +1512,19 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D27" s="8">
-        <v>0.2286</v>
+        <v>8.4959999999999994E-2</v>
       </c>
       <c r="E27" s="8">
-        <v>5.4550000000000001E-2</v>
+        <v>-0.439</v>
       </c>
       <c r="F27" s="8">
-        <v>0.48549999999999999</v>
+        <v>0.59489999999999998</v>
       </c>
       <c r="G27">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="2:7">
@@ -1500,38 +1532,118 @@
         <v>47</v>
       </c>
       <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0.1037</v>
+      </c>
+      <c r="E28" s="8">
+        <v>5.2440000000000001E-2</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.1555</v>
+      </c>
+      <c r="G28">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0.1905</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="G29">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="8">
+        <v>0.34770000000000001</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0.29160000000000003</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.42420000000000002</v>
+      </c>
+      <c r="G30">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="8">
+        <v>0.2286</v>
+      </c>
+      <c r="E31" s="8">
+        <v>5.4550000000000001E-2</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.48549999999999999</v>
+      </c>
+      <c r="G31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D32" s="8">
         <v>0.15620000000000001</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E32" s="8">
         <v>-0.67359999999999998</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F32" s="8">
         <v>0.87460000000000004</v>
       </c>
-      <c r="G28">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="G32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D33" s="7">
         <v>0.40229999999999999</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E33" s="7">
         <v>0.30930000000000002</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F33" s="7">
         <v>0.51700000000000002</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G33" s="4">
         <v>45</v>
       </c>
     </row>
@@ -1543,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B05918F-887D-3446-BE2D-BB31DE00B69A}">
-  <dimension ref="A2:F162"/>
+  <dimension ref="A2:F169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1557,85 +1669,76 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="17" thickBot="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="17" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0.61499999999999999</v>
-      </c>
-      <c r="F3" t="s">
-        <v>122</v>
+      <c r="A3" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="31">
+        <v>0.39400000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="8">
-        <v>0.57799999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="8">
-        <v>-4.0000000000000001E-3</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18">
-      <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="8">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18">
+      <c r="A4" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="31">
+        <v>0.49199999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="31">
+        <v>0.35299999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="32">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1643,13 +1746,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D7" s="8">
-        <v>-2E-3</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>120</v>
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="F7" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1660,13 +1763,13 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D8" s="8">
-        <v>0.23300000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>0.57799999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1674,13 +1777,16 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D9" s="8">
-        <v>0.58799999999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1688,13 +1794,16 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D10" s="8">
-        <v>-8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -1702,24 +1811,27 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D11" s="8">
-        <v>0.49199999999999999</v>
+        <v>-2E-3</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="7">
-        <v>-2E-3</v>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.23300000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1727,13 +1839,13 @@
         <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D13" s="8">
-        <v>0.64400000000000002</v>
+        <v>0.58799999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1741,13 +1853,13 @@
         <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D14" s="8">
-        <v>0.86799999999999999</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1755,13 +1867,13 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D15" s="8">
-        <v>0.21299999999999999</v>
+        <v>0.49199999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1769,13 +1881,13 @@
         <v>47</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D16" s="7">
-        <v>6.0999999999999999E-2</v>
+        <v>-2E-3</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1783,13 +1895,13 @@
         <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D17" s="8">
-        <v>9.5000000000000001E-2</v>
+        <v>0.64400000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1797,13 +1909,13 @@
         <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D18" s="8">
-        <v>0.245</v>
+        <v>0.86799999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1811,27 +1923,27 @@
         <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
         <v>65</v>
       </c>
       <c r="D19" s="8">
-        <v>7.0999999999999994E-2</v>
+        <v>0.21299999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>47</v>
       </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="8">
-        <v>6.0000000000000001E-3</v>
+      <c r="B20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="7">
+        <v>6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1842,10 +1954,10 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D21" s="8">
-        <v>9.1999999999999998E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1856,10 +1968,10 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D22" s="8">
-        <v>-3.0000000000000001E-3</v>
+        <v>0.245</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1870,10 +1982,10 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D23" s="8">
-        <v>3.5999999999999997E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1884,10 +1996,10 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D24" s="8">
-        <v>-3.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1898,80 +2010,80 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D25" s="8">
-        <v>0.40699999999999997</v>
+        <v>9.1999999999999998E-2</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="7">
-        <v>0.20300000000000001</v>
+      <c r="C26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="8">
+        <v>-3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>9</v>
+      <c r="B27" t="s">
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D27" s="8">
-        <v>0.27300000000000002</v>
+        <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>9</v>
+      <c r="B28" t="s">
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D28" s="8">
-        <v>0.80300000000000005</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>9</v>
+      <c r="B29" t="s">
+        <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D29" s="8">
-        <v>4.8000000000000001E-2</v>
+        <v>0.40699999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="8">
-        <v>0.33200000000000002</v>
+      <c r="B30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0.20300000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1982,10 +2094,10 @@
         <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D31" s="8">
-        <v>0.41299999999999998</v>
+        <v>0.27300000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1996,10 +2108,10 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="D32" s="8">
-        <v>8.9999999999999993E-3</v>
+        <v>0.80300000000000005</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2010,10 +2122,10 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D33" s="8">
-        <v>0.28399999999999997</v>
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2024,24 +2136,24 @@
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D34" s="8">
-        <v>0.50700000000000001</v>
+        <v>0.33200000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="7">
-        <v>0.14199999999999999</v>
+      <c r="C35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="8">
+        <v>0.41299999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2049,13 +2161,13 @@
         <v>47</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
         <v>65</v>
       </c>
       <c r="D36" s="8">
-        <v>-0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2063,41 +2175,41 @@
         <v>47</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D37" s="8">
-        <v>4.8000000000000001E-2</v>
+        <v>0.28399999999999997</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" s="7">
-        <v>7.6999999999999999E-2</v>
+      <c r="B38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="8">
+        <v>0.50700000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>47</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="17">
-        <v>1.2E-2</v>
+      <c r="B39" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0.14199999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2105,83 +2217,83 @@
         <v>47</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D40" s="6">
-        <v>0.192</v>
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="8">
+        <v>-0.01</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" s="7">
-        <v>0.249</v>
+      <c r="B41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="8">
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" t="s">
-        <v>65</v>
-      </c>
-      <c r="D42" s="8">
-        <v>0.11</v>
+      <c r="B42" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" s="7">
+        <v>7.6999999999999999E-2</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" s="8">
-        <v>0.21099999999999999</v>
+      <c r="B43" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="14">
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>47</v>
       </c>
-      <c r="B44" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D44" s="7">
-        <v>0.19600000000000001</v>
+      <c r="B44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="6">
+        <v>0.192</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" t="s">
-        <v>87</v>
-      </c>
-      <c r="D45" s="8">
-        <v>-7.0000000000000001E-3</v>
+      <c r="B45" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" s="7">
+        <v>0.249</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2189,41 +2301,41 @@
         <v>47</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="D46" s="8">
-        <v>8.3000000000000004E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" s="7">
-        <v>0.11</v>
+      <c r="B47" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" s="8">
+        <v>0.21099999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" t="s">
-        <v>90</v>
-      </c>
-      <c r="D48" s="8">
-        <v>7.9000000000000001E-2</v>
+      <c r="B48" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" s="7">
+        <v>0.19600000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2231,13 +2343,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D49" s="8">
-        <v>0.153</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2245,41 +2357,41 @@
         <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D50" s="8">
-        <v>0.158</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51" t="s">
-        <v>93</v>
-      </c>
-      <c r="D51" s="8">
-        <v>0.21</v>
+      <c r="B51" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="7">
+        <v>0.11</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D52" s="7">
-        <v>3.1E-2</v>
+      <c r="C52" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="8">
+        <v>7.9000000000000001E-2</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2287,13 +2399,13 @@
         <v>47</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="C53" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D53" s="8">
-        <v>9.4E-2</v>
+        <v>0.153</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2301,13 +2413,13 @@
         <v>47</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="C54" t="s">
         <v>92</v>
       </c>
       <c r="D54" s="8">
-        <v>-1.7999999999999999E-2</v>
+        <v>0.158</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2315,27 +2427,27 @@
         <v>47</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="C55" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="D55" s="8">
-        <v>2.5000000000000001E-2</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C56" t="s">
-        <v>96</v>
-      </c>
-      <c r="D56" s="8">
-        <v>0.27500000000000002</v>
+      <c r="B56" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" s="7">
+        <v>3.1E-2</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2346,10 +2458,10 @@
         <v>100</v>
       </c>
       <c r="C57" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D57" s="8">
-        <v>0.32900000000000001</v>
+        <v>9.4E-2</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2360,24 +2472,24 @@
         <v>100</v>
       </c>
       <c r="C58" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D58" s="8">
-        <v>0.32500000000000001</v>
+        <v>-1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>47</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D59" s="7">
-        <v>0.373</v>
+      <c r="C59" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59" s="8">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2385,13 +2497,13 @@
         <v>47</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D60" s="8">
-        <v>0.17</v>
+        <v>0.27500000000000002</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2399,13 +2511,13 @@
         <v>47</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D61" s="8">
-        <v>0.52</v>
+        <v>0.32900000000000001</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2413,27 +2525,27 @@
         <v>47</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C62" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D62" s="8">
-        <v>0.115</v>
+        <v>0.32500000000000001</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>47</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C63" t="s">
-        <v>104</v>
-      </c>
-      <c r="D63" s="8">
-        <v>0.34799999999999998</v>
+      <c r="B63" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D63" s="7">
+        <v>0.373</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2444,10 +2556,10 @@
         <v>109</v>
       </c>
       <c r="C64" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="D64" s="8">
-        <v>-7.0000000000000001E-3</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2458,10 +2570,10 @@
         <v>109</v>
       </c>
       <c r="C65" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D65" s="8">
-        <v>0.375</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2472,10 +2584,10 @@
         <v>109</v>
       </c>
       <c r="C66" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D66" s="8">
-        <v>0.35099999999999998</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2486,24 +2598,24 @@
         <v>109</v>
       </c>
       <c r="C67" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D67" s="8">
-        <v>-1.2E-2</v>
+        <v>0.34799999999999998</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>47</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B68" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C68" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D68" s="7">
-        <v>-0.03</v>
+      <c r="C68" t="s">
+        <v>65</v>
+      </c>
+      <c r="D68" s="8">
+        <v>-7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2511,13 +2623,13 @@
         <v>47</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="C69" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D69" s="8">
-        <v>0.14099999999999999</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2525,13 +2637,13 @@
         <v>47</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="C70" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="D70" s="8">
-        <v>8.5999999999999993E-2</v>
+        <v>0.35099999999999998</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2539,27 +2651,27 @@
         <v>47</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="C71" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D71" s="8">
-        <v>0.307</v>
+        <v>-1.2E-2</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>47</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C72" t="s">
-        <v>112</v>
-      </c>
-      <c r="D72" s="8">
-        <v>0.48</v>
+      <c r="B72" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D72" s="7">
+        <v>-0.03</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2570,24 +2682,24 @@
         <v>17</v>
       </c>
       <c r="C73" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="D73" s="8">
-        <v>1.7999999999999999E-2</v>
+        <v>0.14099999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>47</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B74" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C74" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D74" s="7">
-        <v>0.12</v>
+      <c r="C74" t="s">
+        <v>77</v>
+      </c>
+      <c r="D74" s="8">
+        <v>8.5999999999999993E-2</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2595,27 +2707,27 @@
         <v>47</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C75" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="D75" s="8">
-        <v>0.29399999999999998</v>
+        <v>0.307</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D76" s="7">
-        <v>0.29399999999999998</v>
+      <c r="B76" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76" t="s">
+        <v>112</v>
+      </c>
+      <c r="D76" s="8">
+        <v>0.48</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2623,27 +2735,27 @@
         <v>47</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C77" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
       <c r="D77" s="8">
-        <v>0.42</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>47</v>
       </c>
-      <c r="B78" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C78" t="s">
-        <v>114</v>
-      </c>
-      <c r="D78" s="8">
-        <v>0.14499999999999999</v>
+      <c r="B78" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D78" s="7">
+        <v>0.12</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2651,125 +2763,125 @@
         <v>47</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C79" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="D79" s="8">
-        <v>0.57599999999999996</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="17" thickBot="1">
-      <c r="A80" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B80" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C80" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="D80" s="23">
-        <v>0.32200000000000001</v>
+        <v>0.29399999999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>47</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D80" s="7">
+        <v>0.29399999999999998</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>5</v>
-      </c>
-      <c r="B81" t="s">
-        <v>6</v>
+        <v>47</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C81" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D81" s="8">
-        <v>0.60799999999999998</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>5</v>
-      </c>
-      <c r="B82" t="s">
-        <v>6</v>
+        <v>47</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C82" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="D82" s="8">
-        <v>0.53700000000000003</v>
+        <v>0.14499999999999999</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>5</v>
-      </c>
-      <c r="B83" t="s">
-        <v>6</v>
+        <v>47</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C83" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
       <c r="D83" s="8">
-        <v>-4.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" t="s">
-        <v>5</v>
-      </c>
-      <c r="B84" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84" t="s">
-        <v>54</v>
-      </c>
-      <c r="D84" s="8">
-        <v>-2E-3</v>
+        <v>0.57599999999999996</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="17" thickBot="1">
+      <c r="A84" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B84" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D84" s="20">
+        <v>0.32200000000000001</v>
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" t="s">
-        <v>5</v>
-      </c>
-      <c r="B85" t="s">
-        <v>6</v>
-      </c>
-      <c r="C85" t="s">
-        <v>55</v>
-      </c>
-      <c r="D85" s="8">
-        <v>-2E-3</v>
+      <c r="A85" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D85" s="6">
+        <v>0.47</v>
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" t="s">
-        <v>5</v>
-      </c>
-      <c r="B86" t="s">
-        <v>6</v>
-      </c>
-      <c r="C86" t="s">
-        <v>56</v>
-      </c>
-      <c r="D86" s="8">
-        <v>0.123</v>
+      <c r="A86" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D86" s="6">
+        <v>0.50600000000000001</v>
       </c>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" t="s">
-        <v>5</v>
-      </c>
-      <c r="B87" t="s">
-        <v>6</v>
-      </c>
-      <c r="C87" t="s">
-        <v>57</v>
-      </c>
-      <c r="D87" s="8">
-        <v>0.376</v>
+      <c r="A87" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D87" s="7">
+        <v>0.499</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2780,10 +2892,10 @@
         <v>6</v>
       </c>
       <c r="C88" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D88" s="8">
-        <v>0.18</v>
+        <v>0.60799999999999998</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2794,23 +2906,23 @@
         <v>6</v>
       </c>
       <c r="C89" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D89" s="8">
-        <v>0.111</v>
+        <v>0.53700000000000003</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>5</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" t="s">
         <v>6</v>
       </c>
-      <c r="C90" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D90" s="7">
+      <c r="C90" t="s">
+        <v>53</v>
+      </c>
+      <c r="D90" s="8">
         <v>-4.0000000000000001E-3</v>
       </c>
     </row>
@@ -2819,13 +2931,13 @@
         <v>5</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C91" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D91" s="8">
-        <v>0.56999999999999995</v>
+        <v>-2E-3</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2833,13 +2945,13 @@
         <v>5</v>
       </c>
       <c r="B92" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C92" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D92" s="8">
-        <v>0.621</v>
+        <v>-2E-3</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2847,27 +2959,27 @@
         <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C93" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D93" s="8">
-        <v>6.8000000000000005E-2</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>5</v>
       </c>
-      <c r="B94" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D94" s="7">
-        <v>0.17499999999999999</v>
+      <c r="B94" t="s">
+        <v>6</v>
+      </c>
+      <c r="C94" t="s">
+        <v>57</v>
+      </c>
+      <c r="D94" s="8">
+        <v>0.376</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2875,13 +2987,13 @@
         <v>5</v>
       </c>
       <c r="B95" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C95" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D95" s="8">
-        <v>7.0000000000000007E-2</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2889,27 +3001,27 @@
         <v>5</v>
       </c>
       <c r="B96" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C96" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D96" s="8">
-        <v>0.13100000000000001</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>5</v>
       </c>
-      <c r="B97" t="s">
-        <v>8</v>
-      </c>
-      <c r="C97" t="s">
-        <v>65</v>
-      </c>
-      <c r="D97" s="8">
-        <v>5.3999999999999999E-2</v>
+      <c r="B97" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D97" s="7">
+        <v>-4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2917,13 +3029,13 @@
         <v>5</v>
       </c>
       <c r="B98" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D98" s="8">
-        <v>6.0999999999999999E-2</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2931,13 +3043,13 @@
         <v>5</v>
       </c>
       <c r="B99" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C99" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D99" s="8">
-        <v>0.13800000000000001</v>
+        <v>0.621</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2945,27 +3057,27 @@
         <v>5</v>
       </c>
       <c r="B100" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C100" t="s">
-        <v>58</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>117</v>
+        <v>65</v>
+      </c>
+      <c r="D100" s="8">
+        <v>6.8000000000000005E-2</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>5</v>
       </c>
-      <c r="B101" t="s">
-        <v>8</v>
-      </c>
-      <c r="C101" t="s">
-        <v>71</v>
-      </c>
-      <c r="D101" s="8">
-        <v>7.0000000000000007E-2</v>
+      <c r="B101" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D101" s="7">
+        <v>0.17499999999999999</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2976,10 +3088,10 @@
         <v>8</v>
       </c>
       <c r="C102" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D102" s="8">
-        <v>-6.0000000000000001E-3</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2990,122 +3102,122 @@
         <v>8</v>
       </c>
       <c r="C103" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D103" s="8">
-        <v>0.46899999999999997</v>
+        <v>0.13100000000000001</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>5</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" t="s">
         <v>8</v>
       </c>
-      <c r="C104" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D104" s="7">
-        <v>0.192</v>
+      <c r="C104" t="s">
+        <v>65</v>
+      </c>
+      <c r="D104" s="8">
+        <v>5.3999999999999999E-2</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>5</v>
       </c>
-      <c r="B105" s="5" t="s">
-        <v>9</v>
+      <c r="B105" t="s">
+        <v>8</v>
       </c>
       <c r="C105" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D105" s="8">
-        <v>0.185</v>
+        <v>6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>5</v>
       </c>
-      <c r="B106" s="5" t="s">
-        <v>9</v>
+      <c r="B106" t="s">
+        <v>8</v>
       </c>
       <c r="C106" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D106" s="8">
-        <v>0.55700000000000005</v>
+        <v>0.13800000000000001</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>5</v>
       </c>
-      <c r="B107" s="5" t="s">
-        <v>9</v>
+      <c r="B107" t="s">
+        <v>8</v>
       </c>
       <c r="C107" t="s">
-        <v>77</v>
-      </c>
-      <c r="D107" s="8">
-        <v>0.26</v>
+        <v>58</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>5</v>
       </c>
-      <c r="B108" s="5" t="s">
-        <v>9</v>
+      <c r="B108" t="s">
+        <v>8</v>
       </c>
       <c r="C108" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D108" s="8">
-        <v>0.78400000000000003</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>5</v>
       </c>
-      <c r="B109" s="5" t="s">
-        <v>9</v>
+      <c r="B109" t="s">
+        <v>8</v>
       </c>
       <c r="C109" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D109" s="8">
-        <v>0.46700000000000003</v>
+        <v>-6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>5</v>
       </c>
-      <c r="B110" s="5" t="s">
-        <v>9</v>
+      <c r="B110" t="s">
+        <v>8</v>
       </c>
       <c r="C110" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D110" s="8">
-        <v>0.13800000000000001</v>
+        <v>0.46899999999999997</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>5</v>
       </c>
-      <c r="B111" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C111" t="s">
-        <v>80</v>
-      </c>
-      <c r="D111" s="8">
-        <v>0.22600000000000001</v>
+      <c r="B111" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D111" s="7">
+        <v>0.192</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -3116,24 +3228,24 @@
         <v>9</v>
       </c>
       <c r="C112" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D112" s="8">
-        <v>0.58699999999999997</v>
+        <v>0.185</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>5</v>
       </c>
-      <c r="B113" s="10" t="s">
+      <c r="B113" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C113" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D113" s="7">
-        <v>-1.2999999999999999E-2</v>
+      <c r="C113" t="s">
+        <v>76</v>
+      </c>
+      <c r="D113" s="8">
+        <v>0.55700000000000005</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -3141,13 +3253,13 @@
         <v>5</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C114" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="D114" s="8">
-        <v>0.105</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -3155,41 +3267,41 @@
         <v>5</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C115" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D115" s="8">
-        <v>4.4999999999999998E-2</v>
+        <v>0.78400000000000003</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>5</v>
       </c>
-      <c r="B116" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D116" s="7">
-        <v>-3.0000000000000001E-3</v>
+      <c r="B116" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C116" t="s">
+        <v>79</v>
+      </c>
+      <c r="D116" s="8">
+        <v>0.46700000000000003</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>5</v>
       </c>
-      <c r="B117" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C117" s="16" t="s">
+      <c r="B117" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C117" t="s">
         <v>65</v>
       </c>
       <c r="D117" s="8">
-        <v>8.5999999999999993E-2</v>
+        <v>0.13800000000000001</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -3197,41 +3309,41 @@
         <v>5</v>
       </c>
       <c r="B118" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>83</v>
+        <v>9</v>
+      </c>
+      <c r="C118" t="s">
+        <v>80</v>
       </c>
       <c r="D118" s="8">
-        <v>0.40799999999999997</v>
+        <v>0.22600000000000001</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>5</v>
       </c>
-      <c r="B119" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D119" s="7">
-        <v>0.52500000000000002</v>
+      <c r="B119" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C119" t="s">
+        <v>81</v>
+      </c>
+      <c r="D119" s="8">
+        <v>0.58699999999999997</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>5</v>
       </c>
-      <c r="B120" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C120" t="s">
-        <v>65</v>
-      </c>
-      <c r="D120" s="8">
-        <v>0.152</v>
+      <c r="B120" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D120" s="7">
+        <v>-1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -3239,55 +3351,55 @@
         <v>5</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C121" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="D121" s="8">
-        <v>0.18099999999999999</v>
+        <v>0.105</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>5</v>
       </c>
-      <c r="B122" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D122" s="7">
-        <v>0.13200000000000001</v>
+      <c r="B122" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C122" t="s">
+        <v>83</v>
+      </c>
+      <c r="D122" s="8">
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>5</v>
       </c>
-      <c r="B123" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C123" t="s">
-        <v>87</v>
-      </c>
-      <c r="D123" s="8">
-        <v>6.9000000000000006E-2</v>
+      <c r="B123" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D123" s="7">
+        <v>-3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>5</v>
       </c>
-      <c r="B124" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C124" t="s">
-        <v>88</v>
+      <c r="B124" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C124" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="D124" s="8">
-        <v>8.2000000000000003E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3295,13 +3407,13 @@
         <v>5</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C125" t="s">
-        <v>65</v>
+        <v>11</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="D125" s="8">
-        <v>-2E-3</v>
+        <v>0.40799999999999997</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3309,27 +3421,27 @@
         <v>5</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D126" s="7">
-        <v>-5.0000000000000001E-3</v>
+        <v>0.52500000000000002</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>5</v>
       </c>
-      <c r="B127" s="11" t="s">
-        <v>14</v>
+      <c r="B127" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C127" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="D127" s="8">
-        <v>0.11</v>
+        <v>0.152</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3337,27 +3449,27 @@
         <v>5</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C128" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D128" s="8">
-        <v>0.22800000000000001</v>
+        <v>0.18099999999999999</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>5</v>
       </c>
-      <c r="B129" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C129" t="s">
-        <v>92</v>
-      </c>
-      <c r="D129" s="8">
-        <v>0.21299999999999999</v>
+      <c r="B129" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D129" s="7">
+        <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3365,27 +3477,27 @@
         <v>5</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C130" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D130" s="8">
-        <v>0.315</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>5</v>
       </c>
-      <c r="B131" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D131" s="7">
-        <v>0.14000000000000001</v>
+      <c r="B131" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C131" t="s">
+        <v>88</v>
+      </c>
+      <c r="D131" s="8">
+        <v>8.2000000000000003E-2</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3393,41 +3505,41 @@
         <v>5</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="C132" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="D132" s="8">
-        <v>0.29899999999999999</v>
+        <v>-2E-3</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
         <v>5</v>
       </c>
-      <c r="B133" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C133" t="s">
-        <v>92</v>
-      </c>
-      <c r="D133" s="8" t="s">
-        <v>117</v>
+      <c r="B133" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D133" s="7">
+        <v>-5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>5</v>
       </c>
-      <c r="B134" s="5" t="s">
-        <v>100</v>
+      <c r="B134" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="C134" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="D134" s="8">
-        <v>5.0999999999999997E-2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3435,13 +3547,13 @@
         <v>5</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="C135" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D135" s="8">
-        <v>6.4000000000000001E-2</v>
+        <v>0.22800000000000001</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3449,13 +3561,13 @@
         <v>5</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="C136" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D136" s="8">
-        <v>0.38500000000000001</v>
+        <v>0.21299999999999999</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -3463,13 +3575,13 @@
         <v>5</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="C137" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D137" s="8">
-        <v>0.49099999999999999</v>
+        <v>0.315</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3477,13 +3589,13 @@
         <v>5</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D138" s="7">
-        <v>0.48799999999999999</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3491,13 +3603,13 @@
         <v>5</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C139" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D139" s="8">
-        <v>0.14000000000000001</v>
+        <v>0.29899999999999999</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3505,13 +3617,13 @@
         <v>5</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C140" t="s">
-        <v>102</v>
-      </c>
-      <c r="D140" s="8">
-        <v>0.53800000000000003</v>
+        <v>92</v>
+      </c>
+      <c r="D140" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3519,13 +3631,13 @@
         <v>5</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C141" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
       <c r="D141" s="8">
-        <v>0.40500000000000003</v>
+        <v>5.0999999999999997E-2</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3533,13 +3645,13 @@
         <v>5</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C142" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D142" s="8">
-        <v>0.54300000000000004</v>
+        <v>6.4000000000000001E-2</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -3547,13 +3659,13 @@
         <v>5</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C143" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="D143" s="8">
-        <v>-6.0000000000000001E-3</v>
+        <v>0.38500000000000001</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -3561,27 +3673,27 @@
         <v>5</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C144" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D144" s="8">
-        <v>0.23300000000000001</v>
+        <v>0.49099999999999999</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
         <v>5</v>
       </c>
-      <c r="B145" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C145" t="s">
-        <v>106</v>
-      </c>
-      <c r="D145" s="8">
-        <v>0.38</v>
+      <c r="B145" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D145" s="7">
+        <v>0.48799999999999999</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -3592,24 +3704,24 @@
         <v>109</v>
       </c>
       <c r="C146" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D146" s="8">
-        <v>6.6000000000000003E-2</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
         <v>5</v>
       </c>
-      <c r="B147" s="10" t="s">
+      <c r="B147" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C147" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D147" s="7">
-        <v>-1.7000000000000001E-2</v>
+      <c r="C147" t="s">
+        <v>102</v>
+      </c>
+      <c r="D147" s="8">
+        <v>0.53800000000000003</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3617,13 +3729,13 @@
         <v>5</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="C148" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D148" s="8">
-        <v>4.1000000000000002E-2</v>
+        <v>0.40500000000000003</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3631,13 +3743,13 @@
         <v>5</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="C149" t="s">
-        <v>77</v>
-      </c>
-      <c r="D149" s="8" t="s">
-        <v>117</v>
+        <v>104</v>
+      </c>
+      <c r="D149" s="8">
+        <v>0.54300000000000004</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3645,13 +3757,13 @@
         <v>5</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="C150" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="D150" s="8">
-        <v>0.29699999999999999</v>
+        <v>-6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3659,13 +3771,13 @@
         <v>5</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="C151" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D151" s="8">
-        <v>0.55900000000000005</v>
+        <v>0.23300000000000001</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -3673,41 +3785,41 @@
         <v>5</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="C152" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="D152" s="8">
-        <v>3.9E-2</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
         <v>5</v>
       </c>
-      <c r="B153" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C153" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D153" s="7">
-        <v>0.105</v>
+      <c r="B153" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C153" t="s">
+        <v>107</v>
+      </c>
+      <c r="D153" s="8">
+        <v>6.6000000000000003E-2</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
         <v>5</v>
       </c>
-      <c r="B154" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C154" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D154" s="8">
-        <v>-1.4E-2</v>
+      <c r="B154" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D154" s="7">
+        <v>-1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3715,27 +3827,27 @@
         <v>5</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C155" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="D155" s="8">
-        <v>8.5999999999999993E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
         <v>5</v>
       </c>
-      <c r="B156" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C156" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D156" s="7">
-        <v>0.23100000000000001</v>
+      <c r="B156" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C156" t="s">
+        <v>77</v>
+      </c>
+      <c r="D156" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -3743,13 +3855,13 @@
         <v>5</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C157" s="5" t="s">
-        <v>91</v>
+        <v>17</v>
+      </c>
+      <c r="C157" t="s">
+        <v>111</v>
       </c>
       <c r="D157" s="8">
-        <v>-3.0000000000000001E-3</v>
+        <v>0.29699999999999999</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -3757,13 +3869,13 @@
         <v>5</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C158" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="D158" s="8">
-        <v>0.28999999999999998</v>
+        <v>0.55900000000000005</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3771,27 +3883,27 @@
         <v>5</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C159" t="s">
         <v>65</v>
       </c>
       <c r="D159" s="8">
-        <v>-6.0000000000000001E-3</v>
+        <v>3.9E-2</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
         <v>5</v>
       </c>
-      <c r="B160" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C160" t="s">
-        <v>114</v>
-      </c>
-      <c r="D160" s="8">
-        <v>0.27700000000000002</v>
+      <c r="B160" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D160" s="7">
+        <v>0.105</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -3799,26 +3911,124 @@
         <v>5</v>
       </c>
       <c r="B161" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D161" s="8">
+        <v>-1.4E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" t="s">
+        <v>5</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C162" t="s">
+        <v>85</v>
+      </c>
+      <c r="D162" s="8">
+        <v>8.5999999999999993E-2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" t="s">
+        <v>5</v>
+      </c>
+      <c r="B163" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C163" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D163" s="7">
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" t="s">
+        <v>5</v>
+      </c>
+      <c r="B164" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C164" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D164" s="8">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" t="s">
+        <v>5</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C165" t="s">
+        <v>92</v>
+      </c>
+      <c r="D165" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" t="s">
+        <v>5</v>
+      </c>
+      <c r="B166" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C166" t="s">
+        <v>65</v>
+      </c>
+      <c r="D166" s="8">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" t="s">
+        <v>5</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C167" t="s">
+        <v>114</v>
+      </c>
+      <c r="D167" s="8">
+        <v>0.27700000000000002</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" t="s">
+        <v>5</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C168" t="s">
         <v>115</v>
       </c>
-      <c r="D161" s="8">
+      <c r="D168" s="8">
         <v>0.54400000000000004</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="17" thickBot="1">
-      <c r="A162" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B162" s="22" t="s">
+    <row r="169" spans="1:4" ht="17" thickBot="1">
+      <c r="A169" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C162" s="21" t="s">
+      <c r="C169" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D162" s="23">
+      <c r="D169" s="20">
         <v>0.4</v>
       </c>
     </row>
@@ -3831,7 +4041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFB3FF2-77B5-D244-AC2F-4BD444475F41}">
   <dimension ref="B2:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+    <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
@@ -3871,10 +4081,10 @@
       </c>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -3897,8 +4107,8 @@
       </c>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
@@ -3916,8 +4126,8 @@
       </c>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="3" t="s">
         <v>24</v>
       </c>
@@ -3935,8 +4145,8 @@
       </c>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
@@ -3954,8 +4164,8 @@
       </c>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="4" t="s">
         <v>26</v>
       </c>
@@ -3974,8 +4184,8 @@
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="12"/>
-      <c r="C8" s="14" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="24" t="s">
         <v>46</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -3998,8 +4208,8 @@
       </c>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="5" t="s">
         <v>30</v>
       </c>
@@ -4017,8 +4227,8 @@
       </c>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="5" t="s">
         <v>31</v>
       </c>
@@ -4036,8 +4246,8 @@
       </c>
     </row>
     <row r="11" spans="2:11">
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="5" t="s">
         <v>34</v>
       </c>
@@ -4055,8 +4265,8 @@
       </c>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="5" t="s">
         <v>35</v>
       </c>
@@ -4074,8 +4284,8 @@
       </c>
     </row>
     <row r="13" spans="2:11">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="5" t="s">
         <v>32</v>
       </c>
@@ -4093,8 +4303,8 @@
       </c>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="5" t="s">
         <v>33</v>
       </c>
@@ -4112,8 +4322,8 @@
       </c>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="5" t="s">
         <v>36</v>
       </c>
@@ -4131,8 +4341,8 @@
       </c>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="5" t="s">
         <v>37</v>
       </c>
@@ -4150,8 +4360,8 @@
       </c>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="5" t="s">
         <v>38</v>
       </c>
@@ -4169,8 +4379,8 @@
       </c>
     </row>
     <row r="18" spans="2:9">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="5" t="s">
         <v>39</v>
       </c>
@@ -4188,8 +4398,8 @@
       </c>
     </row>
     <row r="19" spans="2:9">
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="5" t="s">
         <v>40</v>
       </c>
@@ -4207,8 +4417,8 @@
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="5" t="s">
         <v>41</v>
       </c>
@@ -4226,8 +4436,8 @@
       </c>
     </row>
     <row r="21" spans="2:9">
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="5" t="s">
         <v>42</v>
       </c>
@@ -4245,8 +4455,8 @@
       </c>
     </row>
     <row r="22" spans="2:9">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
       <c r="D22" s="5" t="s">
         <v>43</v>
       </c>
@@ -4264,8 +4474,8 @@
       </c>
     </row>
     <row r="23" spans="2:9">
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="5" t="s">
         <v>44</v>
       </c>
@@ -4283,8 +4493,8 @@
       </c>
     </row>
     <row r="24" spans="2:9">
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="10" t="s">
         <v>45</v>
       </c>
@@ -4305,10 +4515,10 @@
       </c>
     </row>
     <row r="25" spans="2:9">
-      <c r="B25" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="12" t="s">
+      <c r="B25" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="22" t="s">
         <v>28</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -4328,8 +4538,8 @@
       </c>
     </row>
     <row r="26" spans="2:9">
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="3" t="s">
         <v>23</v>
       </c>
@@ -4347,8 +4557,8 @@
       </c>
     </row>
     <row r="27" spans="2:9">
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="3" t="s">
         <v>24</v>
       </c>
@@ -4366,8 +4576,8 @@
       </c>
     </row>
     <row r="28" spans="2:9">
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="3" t="s">
         <v>25</v>
       </c>
@@ -4385,8 +4595,8 @@
       </c>
     </row>
     <row r="29" spans="2:9">
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="4" t="s">
         <v>26</v>
       </c>
@@ -4404,23 +4614,23 @@
       </c>
     </row>
     <row r="30" spans="2:9">
-      <c r="B30" s="12"/>
-      <c r="C30" s="14" t="s">
+      <c r="B30" s="22"/>
+      <c r="C30" s="24" t="s">
         <v>46</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="14">
         <v>0.96399999999999997</v>
       </c>
-      <c r="F30" s="17">
+      <c r="F30" s="14">
         <v>0.94399999999999995</v>
       </c>
-      <c r="G30" s="17">
+      <c r="G30" s="14">
         <v>0.97499999999999998</v>
       </c>
-      <c r="H30" s="18">
+      <c r="H30" s="15">
         <v>50</v>
       </c>
       <c r="I30" t="s">
@@ -4428,8 +4638,8 @@
       </c>
     </row>
     <row r="31" spans="2:9">
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
       <c r="D31" s="5" t="s">
         <v>30</v>
       </c>
@@ -4442,13 +4652,13 @@
       <c r="G31" s="6">
         <v>0.98699999999999999</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="32" spans="2:9">
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="5" t="s">
         <v>31</v>
       </c>
@@ -4461,13 +4671,13 @@
       <c r="G32" s="6">
         <v>1</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="33" spans="2:9">
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
       <c r="D33" s="5" t="s">
         <v>34</v>
       </c>
@@ -4480,13 +4690,13 @@
       <c r="G33" s="6">
         <v>0.96599999999999997</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="2:9">
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="5" t="s">
         <v>35</v>
       </c>
@@ -4499,13 +4709,13 @@
       <c r="G34" s="6">
         <v>0.93899999999999995</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="35" spans="2:9">
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="5" t="s">
         <v>32</v>
       </c>
@@ -4518,13 +4728,13 @@
       <c r="G35" s="6">
         <v>0.82099999999999995</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H35" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="36" spans="2:9">
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="5" t="s">
         <v>33</v>
       </c>
@@ -4537,13 +4747,13 @@
       <c r="G36" s="6">
         <v>0.82099999999999995</v>
       </c>
-      <c r="H36" s="15">
+      <c r="H36" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="37" spans="2:9">
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="5" t="s">
         <v>36</v>
       </c>
@@ -4556,13 +4766,13 @@
       <c r="G37" s="6">
         <v>0.88300000000000001</v>
       </c>
-      <c r="H37" s="15">
+      <c r="H37" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="38" spans="2:9">
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
       <c r="D38" s="5" t="s">
         <v>37</v>
       </c>
@@ -4575,13 +4785,13 @@
       <c r="G38" s="6">
         <v>0.82</v>
       </c>
-      <c r="H38" s="15">
+      <c r="H38" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="2:9">
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
       <c r="D39" s="5" t="s">
         <v>38</v>
       </c>
@@ -4594,13 +4804,13 @@
       <c r="G39" s="6">
         <v>0.83299999999999996</v>
       </c>
-      <c r="H39" s="15">
+      <c r="H39" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="40" spans="2:9">
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
       <c r="D40" s="5" t="s">
         <v>39</v>
       </c>
@@ -4613,13 +4823,13 @@
       <c r="G40" s="6">
         <v>0.78</v>
       </c>
-      <c r="H40" s="15">
+      <c r="H40" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="41" spans="2:9">
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
       <c r="D41" s="5" t="s">
         <v>40</v>
       </c>
@@ -4632,13 +4842,13 @@
       <c r="G41" s="6">
         <v>0.77300000000000002</v>
       </c>
-      <c r="H41" s="15">
+      <c r="H41" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="42" spans="2:9">
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
       <c r="D42" s="5" t="s">
         <v>41</v>
       </c>
@@ -4651,13 +4861,13 @@
       <c r="G42" s="6">
         <v>0.91500000000000004</v>
       </c>
-      <c r="H42" s="15">
+      <c r="H42" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="43" spans="2:9">
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
       <c r="D43" s="5" t="s">
         <v>42</v>
       </c>
@@ -4670,13 +4880,13 @@
       <c r="G43" s="6">
         <v>0.875</v>
       </c>
-      <c r="H43" s="15">
+      <c r="H43" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="44" spans="2:9">
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
       <c r="D44" s="5" t="s">
         <v>43</v>
       </c>
@@ -4689,13 +4899,13 @@
       <c r="G44" s="6">
         <v>0.86</v>
       </c>
-      <c r="H44" s="15">
+      <c r="H44" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="45" spans="2:9">
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
       <c r="D45" s="5" t="s">
         <v>44</v>
       </c>
@@ -4708,13 +4918,13 @@
       <c r="G45" s="6">
         <v>0.86</v>
       </c>
-      <c r="H45" s="15">
+      <c r="H45" s="12">
         <v>50</v>
       </c>
     </row>
     <row r="46" spans="2:9">
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
       <c r="D46" s="10" t="s">
         <v>45</v>
       </c>
@@ -4727,7 +4937,7 @@
       <c r="G46" s="7">
         <v>0.15</v>
       </c>
-      <c r="H46" s="19">
+      <c r="H46" s="16">
         <v>50</v>
       </c>
       <c r="I46" t="s">

</xml_diff>

<commit_message>
Changes to summary stats
Changes to summary stats
</commit_message>
<xml_diff>
--- a/inter_rater_reliability_results.xlsx
+++ b/inter_rater_reliability_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Projects/CoMSAfrica/Geneva/Data analysis/CoMSA_stats/comsafrica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0D330A-BD8E-AF44-A477-DFC1F9B62EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46974BEB-7637-1746-81A2-DF7E9E7E65AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{FB42F035-823F-2442-986B-DBADFA145460}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{FB42F035-823F-2442-986B-DBADFA145460}"/>
   </bookViews>
   <sheets>
     <sheet name="Count and continuous_analyst" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="135">
   <si>
     <t>Variable</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t>Bifacial shaping</t>
+  </si>
+  <si>
+    <t>Platform thickness impact point</t>
+  </si>
+  <si>
+    <t>Platform thickness mid point</t>
   </si>
 </sst>
 </file>
@@ -537,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -563,23 +569,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -587,6 +578,22 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,10 +719,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1015,11 +1018,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFB3FF2-77B5-D244-AC2F-4BD444475F41}">
-  <dimension ref="B1:J24"/>
+  <dimension ref="B1:J26"/>
   <sheetViews>
-    <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:F24"/>
+    <sheetView tabSelected="1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1040,30 +1043,30 @@
       <c r="H1" s="13"/>
     </row>
     <row r="2" spans="2:10" ht="17" thickBot="1">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="25" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="37" t="s">
         <v>43</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -1086,7 +1089,7 @@
       </c>
     </row>
     <row r="4" spans="2:10">
-      <c r="B4" s="25"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1105,7 +1108,7 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="2:10">
-      <c r="B5" s="25"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="3" t="s">
         <v>28</v>
       </c>
@@ -1127,7 +1130,7 @@
       </c>
     </row>
     <row r="6" spans="2:10">
-      <c r="B6" s="25"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
@@ -1146,7 +1149,7 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" s="25"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="3" t="s">
         <v>32</v>
       </c>
@@ -1165,7 +1168,7 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="25"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="3" t="s">
         <v>29</v>
       </c>
@@ -1184,7 +1187,7 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="25"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="3" t="s">
         <v>30</v>
       </c>
@@ -1203,7 +1206,7 @@
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="B10" s="25"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="3" t="s">
         <v>33</v>
       </c>
@@ -1222,7 +1225,7 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="B11" s="25"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
@@ -1241,7 +1244,7 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:10">
-      <c r="B12" s="25"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
@@ -1260,7 +1263,7 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="2:10">
-      <c r="B13" s="25"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="3" t="s">
         <v>36</v>
       </c>
@@ -1279,7 +1282,7 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="B14" s="25"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="3" t="s">
         <v>37</v>
       </c>
@@ -1298,7 +1301,7 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="2:10">
-      <c r="B15" s="25"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
@@ -1317,7 +1320,7 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="2:10">
-      <c r="B16" s="25"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="3" t="s">
         <v>39</v>
       </c>
@@ -1336,7 +1339,7 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="2:8">
-      <c r="B17" s="25"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="3" t="s">
         <v>40</v>
       </c>
@@ -1355,7 +1358,7 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="2:8">
-      <c r="B18" s="25"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="3" t="s">
         <v>41</v>
       </c>
@@ -1373,128 +1376,166 @@
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="2:8" ht="17" thickBot="1">
-      <c r="B19" s="30"/>
-      <c r="C19" s="14" t="s">
+    <row r="19" spans="2:8">
+      <c r="B19" s="35"/>
+      <c r="C19" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.82</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.86</v>
+      </c>
+      <c r="G19" s="3">
+        <v>99</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="35"/>
+      <c r="C20" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.82</v>
+      </c>
+      <c r="G20" s="3">
+        <v>99</v>
+      </c>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="2:8" ht="17" thickBot="1">
+      <c r="B21" s="36"/>
+      <c r="C21" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D21" s="15">
         <v>0.01</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E21" s="15">
         <v>0</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F21" s="15">
         <v>0.04</v>
       </c>
-      <c r="G19" s="13">
-        <v>99</v>
-      </c>
-      <c r="H19" s="13" t="s">
+      <c r="G21" s="13">
+        <v>99</v>
+      </c>
+      <c r="H21" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="31" t="s">
+    <row r="22" spans="2:8">
+      <c r="B22" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C22" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D22" s="28">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E22" s="28">
         <v>0.47</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F22" s="28">
         <v>0.65</v>
       </c>
-      <c r="G20" s="34">
-        <v>99</v>
-      </c>
-      <c r="H20" s="34"/>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="25"/>
-      <c r="C21" s="1" t="s">
+      <c r="G22" s="29">
+        <v>99</v>
+      </c>
+      <c r="H22" s="29"/>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="35"/>
+      <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D23" s="4">
         <v>0.47</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E23" s="4">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F23" s="4">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G21" s="1">
-        <v>99</v>
-      </c>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="25"/>
-      <c r="C22" s="1" t="s">
+      <c r="G23" s="1">
+        <v>99</v>
+      </c>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="35"/>
+      <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D24" s="4">
         <v>0.47</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E24" s="4">
         <v>0.35</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F24" s="4">
         <v>0.56999999999999995</v>
       </c>
-      <c r="G22" s="1">
-        <v>99</v>
-      </c>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" s="25"/>
-      <c r="C23" s="1" t="s">
+      <c r="G24" s="1">
+        <v>99</v>
+      </c>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="35"/>
+      <c r="C25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D25" s="4">
         <v>0.5</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E25" s="4">
         <v>0.36</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F25" s="4">
         <v>0.61</v>
       </c>
-      <c r="G23" s="1">
-        <v>99</v>
-      </c>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="2:8" ht="17" thickBot="1">
-      <c r="B24" s="30"/>
-      <c r="C24" s="13" t="s">
+      <c r="G25" s="1">
+        <v>99</v>
+      </c>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" ht="17" thickBot="1">
+      <c r="B26" s="36"/>
+      <c r="C26" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D26" s="15">
         <v>0.65</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E26" s="15">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F26" s="15">
         <v>0.72</v>
       </c>
-      <c r="G24" s="13">
-        <v>99</v>
-      </c>
-      <c r="H24" s="13"/>
+      <c r="G26" s="13">
+        <v>99</v>
+      </c>
+      <c r="H26" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="B3:B19"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="B3:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1503,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B1EF2B-FFAB-3D45-A163-BA1A733786C0}">
-  <dimension ref="B2:G25"/>
+  <dimension ref="B2:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F25"/>
+    <sheetView topLeftCell="A9" zoomScale="191" zoomScaleNormal="191" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1524,27 +1565,27 @@
       <c r="G2" s="13"/>
     </row>
     <row r="3" spans="2:7" ht="17" thickBot="1">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="25" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="37" t="s">
         <v>43</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -1564,7 +1605,7 @@
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="25"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1582,7 +1623,7 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="25"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1600,7 +1641,7 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="25"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
@@ -1618,7 +1659,7 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="25"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1636,7 +1677,7 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="25"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="3" t="s">
         <v>29</v>
       </c>
@@ -1654,7 +1695,7 @@
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="25"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="3" t="s">
         <v>30</v>
       </c>
@@ -1672,7 +1713,7 @@
       </c>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="25"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
@@ -1690,7 +1731,7 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="25"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
@@ -1708,7 +1749,7 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="25"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
@@ -1726,7 +1767,7 @@
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="25"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1744,7 +1785,7 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="25"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
@@ -1762,7 +1803,7 @@
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="25"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="3" t="s">
         <v>38</v>
       </c>
@@ -1780,7 +1821,7 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="25"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="3" t="s">
         <v>39</v>
       </c>
@@ -1798,7 +1839,7 @@
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="25"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="3" t="s">
         <v>40</v>
       </c>
@@ -1816,7 +1857,7 @@
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="25"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="3" t="s">
         <v>41</v>
       </c>
@@ -1833,90 +1874,90 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="17" thickBot="1">
-      <c r="B20" s="30"/>
-      <c r="C20" s="14" t="s">
+    <row r="20" spans="2:7">
+      <c r="B20" s="35"/>
+      <c r="C20" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="19">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E20" s="39">
+        <v>0</v>
+      </c>
+      <c r="F20" s="19">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G20" s="3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="35"/>
+      <c r="C21" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="G21" s="3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="17" thickBot="1">
+      <c r="B22" s="36"/>
+      <c r="C22" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D22" s="15">
         <v>0.01</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E22" s="30">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F22" s="15">
         <v>0.03</v>
       </c>
-      <c r="G20" s="13">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="25" t="s">
+      <c r="G22" s="13">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D23" s="4">
         <v>0.03</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E23" s="7">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F23" s="4">
         <v>0.11</v>
       </c>
-      <c r="G21" s="3">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="25"/>
-      <c r="C22" s="1" t="s">
+      <c r="G23" s="3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="35"/>
+      <c r="C24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D24" s="4">
         <v>0.04</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E24" s="4">
         <v>0.01</v>
-      </c>
-      <c r="F22" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="G22" s="3">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="25"/>
-      <c r="C23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="E23" s="7">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F23" s="4">
-        <v>0.06</v>
-      </c>
-      <c r="G23" s="3">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="25"/>
-      <c r="C24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0.03</v>
-      </c>
-      <c r="E24" s="7">
-        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F24" s="4">
         <v>0.1</v>
@@ -1926,27 +1967,63 @@
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="26"/>
-      <c r="C25" s="2" t="s">
+      <c r="B25" s="35"/>
+      <c r="C25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="E25" s="7">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="G25" s="3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="35"/>
+      <c r="C26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="E26" s="7">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="G26" s="3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="38"/>
+      <c r="C27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D27" s="5">
         <v>0.06</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E27" s="5">
         <v>0.01</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F27" s="5">
         <v>0.13</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G27" s="2">
         <v>99</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B4:B20"/>
-    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="B4:B22"/>
+    <mergeCell ref="B23:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1977,19 +2054,19 @@
       <c r="F1" s="13"/>
     </row>
     <row r="2" spans="2:11" ht="17" thickBot="1">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="25" t="s">
         <v>17</v>
       </c>
       <c r="K2" t="s">
@@ -2306,7 +2383,7 @@
       </c>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="29" t="s">
         <v>121</v>
       </c>
       <c r="C3" s="20" t="s">
@@ -2467,7 +2544,7 @@
       <c r="C16" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D16" s="37">
+      <c r="D16" s="32">
         <v>-2E-3</v>
       </c>
     </row>
@@ -2511,7 +2588,7 @@
       <c r="C20" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="38">
+      <c r="D20" s="33">
         <v>-2E-3</v>
       </c>
     </row>
@@ -2555,7 +2632,7 @@
       <c r="C24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="36">
+      <c r="D24" s="31">
         <v>-2E-3</v>
       </c>
     </row>
@@ -2676,7 +2753,7 @@
       <c r="C35" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="38">
+      <c r="D35" s="33">
         <v>-3.0000000000000001E-3</v>
       </c>
     </row>
@@ -3017,7 +3094,7 @@
       <c r="C66" t="s">
         <v>86</v>
       </c>
-      <c r="D66" s="38">
+      <c r="D66" s="33">
         <v>-8.9999999999999993E-3</v>
       </c>
     </row>
@@ -3127,7 +3204,7 @@
       <c r="C76" t="s">
         <v>59</v>
       </c>
-      <c r="D76" s="38">
+      <c r="D76" s="33">
         <v>-7.0000000000000001E-3</v>
       </c>
     </row>
@@ -3292,7 +3369,7 @@
       <c r="C91" t="s">
         <v>59</v>
       </c>
-      <c r="D91" s="38">
+      <c r="D91" s="33">
         <v>-3.0000000000000001E-3</v>
       </c>
     </row>

</xml_diff>